<commit_message>
continue working on the sript
</commit_message>
<xml_diff>
--- a/wex-users.xlsx
+++ b/wex-users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W513032\source\repos\volume testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835B9EB4-B67E-43A3-ADE6-61645F194A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2F34AE-EA1F-4A4C-B431-BDE3D926FF68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="22455" windowHeight="14775" xr2:uid="{6477CD7D-4DAF-4779-A962-006B329B6AD4}"/>
+    <workbookView xWindow="2340" yWindow="1425" windowWidth="22455" windowHeight="14775" xr2:uid="{6477CD7D-4DAF-4779-A962-006B329B6AD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>T_09684202</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>user-name</t>
+  </si>
+  <si>
+    <t>client-id</t>
   </si>
 </sst>
 </file>
@@ -412,102 +415,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A00AD78-E935-4B24-96CD-5AECDB08FF0C}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="16" customWidth="1"/>
+    <col min="1" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9684202</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>1130</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9684204</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>1130</v>
+      </c>
+      <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9684206</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>1130</v>
+      </c>
+      <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9684208</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>1130</v>
+      </c>
+      <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9684210</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
+        <v>1130</v>
+      </c>
+      <c r="C6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9684212</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7">
+        <v>1130</v>
+      </c>
+      <c r="C7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9684214</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8">
+        <v>1130</v>
+      </c>
+      <c r="C8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9684216</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9">
+        <v>1130</v>
+      </c>
+      <c r="C9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9684218</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10">
+        <v>1130</v>
+      </c>
+      <c r="C10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9684220</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11">
+        <v>1130</v>
+      </c>
+      <c r="C11" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some adjustment to the code
</commit_message>
<xml_diff>
--- a/wex-users.xlsx
+++ b/wex-users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W513032\source\repos\volume testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD4EA60-1525-4999-9017-A372870335C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5A02ED-5567-4E39-9407-1955BF1915FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="825" windowWidth="22455" windowHeight="14775" xr2:uid="{6477CD7D-4DAF-4779-A962-006B329B6AD4}"/>
+    <workbookView xWindow="3120" yWindow="825" windowWidth="22455" windowHeight="14775" xr2:uid="{6477CD7D-4DAF-4779-A962-006B329B6AD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>T_09684202</t>
   </si>
@@ -39,25 +39,10 @@
     <t>client-id</t>
   </si>
   <si>
-    <t>T_09684212</t>
-  </si>
-  <si>
-    <t>T_09684208</t>
-  </si>
-  <si>
     <t>T_09684204</t>
   </si>
   <si>
     <t>T_09684206</t>
-  </si>
-  <si>
-    <t>T_09684210</t>
-  </si>
-  <si>
-    <t>T_09684214</t>
-  </si>
-  <si>
-    <t>T_09684216</t>
   </si>
 </sst>
 </file>
@@ -93,8 +78,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -411,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A00AD78-E935-4B24-96CD-5AECDB08FF0C}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +436,7 @@
         <v>1130</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -463,62 +447,7 @@
         <v>1130</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>9684208</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1130</v>
-      </c>
-      <c r="C5" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>9684210</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1130</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>9684212</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1130</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>9684214</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1130</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>9684216</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1130</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding extra information to acel file
</commit_message>
<xml_diff>
--- a/wex-users.xlsx
+++ b/wex-users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W513032\source\repos\volume testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5A02ED-5567-4E39-9407-1955BF1915FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592008E3-00E2-48AE-9BCE-6169E8F8018B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="825" windowWidth="22455" windowHeight="14775" xr2:uid="{6477CD7D-4DAF-4779-A962-006B329B6AD4}"/>
   </bookViews>
@@ -398,7 +398,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added yellow for Llm problems
</commit_message>
<xml_diff>
--- a/wex-users.xlsx
+++ b/wex-users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W513032\source\repos\volume testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6736AF-1782-4DB7-AAB8-CBCCFE587784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589EA0A0-AF4F-415D-9EFE-492B8D9FE532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="22455" windowHeight="14775" xr2:uid="{6477CD7D-4DAF-4779-A962-006B329B6AD4}"/>
+    <workbookView xWindow="1950" yWindow="825" windowWidth="22455" windowHeight="14775" xr2:uid="{6477CD7D-4DAF-4779-A962-006B329B6AD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>T_09684202</t>
   </si>
@@ -49,21 +49,6 @@
   </si>
   <si>
     <t>T_09684210</t>
-  </si>
-  <si>
-    <t>T_09684212</t>
-  </si>
-  <si>
-    <t>T_09684214</t>
-  </si>
-  <si>
-    <t>T_09684216</t>
-  </si>
-  <si>
-    <t>T_09684218</t>
-  </si>
-  <si>
-    <t>T_09684220</t>
   </si>
 </sst>
 </file>
@@ -416,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A00AD78-E935-4B24-96CD-5AECDB08FF0C}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,61 +478,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>9684212</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1130</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>9684214</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1130</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>9684216</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1130</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9684218</v>
-      </c>
-      <c r="B10" s="1">
-        <v>1130</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>9684220</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1130</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>